<commit_message>
Added example pin headers to BOM
</commit_message>
<xml_diff>
--- a/hardware/documentation/reDIP-RIOT-BOM.xlsx
+++ b/hardware/documentation/reDIP-RIOT-BOM.xlsx
@@ -1580,7 +1580,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="142">
   <si>
     <t>Global Part Info</t>
   </si>
@@ -1706,12 +1706,21 @@
     <t>Conn_01x20</t>
   </si>
   <si>
-    <t>CONN HDR ROUND PIN 0.5mm 20 POS .100" GOLD MATING 3.5mm TAIL 3mm</t>
+    <t>CONN HDR CIRCULAR PIN 0.5mm 20 POS .100" GOLD MATING 3mm TAIL 3mm</t>
+  </si>
+  <si>
+    <t>Replacement parts: XKB X5511WV-20-C396D43-1220, other similar hdr circular pin ~0.5mm</t>
   </si>
   <si>
     <t>PinHeader_1x20_P2.54mm_Vertical_Machined</t>
   </si>
   <si>
+    <t>XKB</t>
+  </si>
+  <si>
+    <t>X5511WV-20-C35D35-1000</t>
+  </si>
+  <si>
     <t>R1,R5</t>
   </si>
   <si>
@@ -1979,7 +1988,7 @@
     <t>Prj date:</t>
   </si>
   <si>
-    <t>ti. 03. okt. 2023 kl. 15.57 +0200</t>
+    <t>on. 04. okt. 2023 kl. 15.15 +0200</t>
   </si>
   <si>
     <t>Board Qty:</t>
@@ -1994,7 +2003,7 @@
     <t>$ date:</t>
   </si>
   <si>
-    <t>2023-10-03 16:16:09</t>
+    <t>2023-10-04 15:15:30</t>
   </si>
   <si>
     <t>KiCost® v1.1.18</t>
@@ -2537,10 +2546,10 @@
     <col min="1" max="1" width="11.7109375" customWidth="1"/>
     <col min="2" max="2" width="18.7109375" customWidth="1"/>
     <col min="3" max="3" width="33.7109375" customWidth="1" outlineLevel="2"/>
-    <col min="4" max="4" width="29.7109375" customWidth="1"/>
+    <col min="4" max="4" width="32.7109375" customWidth="1"/>
     <col min="5" max="5" width="33.7109375" customWidth="1" outlineLevel="2"/>
     <col min="6" max="6" width="10.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="19.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="23.7109375" customWidth="1" outlineLevel="1"/>
     <col min="8" max="8" width="9.140625" outlineLevel="1"/>
     <col min="9" max="9" width="22.7109375" customWidth="1"/>
     <col min="10" max="10" width="16.7109375" customWidth="1"/>
@@ -2560,13 +2569,13 @@
   <sheetData>
     <row r="1" spans="1:22">
       <c r="A1" s="1" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="J1" s="3">
         <v>100</v>
@@ -2574,13 +2583,13 @@
     </row>
     <row r="2" spans="1:22">
       <c r="A2" s="1" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="J2" s="4">
         <f>TotalCost/BoardQty</f>
@@ -2589,13 +2598,13 @@
     </row>
     <row r="3" spans="1:22">
       <c r="A3" s="1" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="J3" s="5">
         <f>SUM(J7:J21)</f>
@@ -2620,10 +2629,10 @@
     </row>
     <row r="4" spans="1:22">
       <c r="A4" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:22">
@@ -2640,7 +2649,7 @@
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="8" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
@@ -2648,7 +2657,7 @@
       <c r="O5" s="8"/>
       <c r="P5" s="8"/>
       <c r="Q5" s="9" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="R5" s="9"/>
       <c r="S5" s="9"/>
@@ -2688,40 +2697,40 @@
         <v>10</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="M6" s="10" t="s">
         <v>9</v>
       </c>
       <c r="N6" s="10" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="O6" s="10" t="s">
         <v>10</v>
       </c>
       <c r="P6" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q6" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="Q6" s="10" t="s">
-        <v>91</v>
-      </c>
       <c r="R6" s="10" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="S6" s="10" t="s">
         <v>9</v>
       </c>
       <c r="T6" s="10" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="U6" s="10" t="s">
         <v>10</v>
       </c>
       <c r="V6" s="10" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:22">
@@ -2774,7 +2783,7 @@
         <v>17.66</v>
       </c>
       <c r="P7" s="11" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="Q7" s="11">
         <v>57211</v>
@@ -2792,7 +2801,7 @@
         <v>17.8</v>
       </c>
       <c r="V7" s="11" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:22">
@@ -2845,7 +2854,7 @@
         <v>15.56</v>
       </c>
       <c r="P8" s="11" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="Q8" s="11">
         <v>777764</v>
@@ -2863,7 +2872,7 @@
         <v>10.8</v>
       </c>
       <c r="V8" s="11" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:22">
@@ -2901,7 +2910,7 @@
         <v/>
       </c>
       <c r="Q9" s="14" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="R9" s="11"/>
       <c r="S9" s="12">
@@ -2916,7 +2925,7 @@
         <v/>
       </c>
       <c r="V9" s="11" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="45" customHeight="1">
@@ -2969,7 +2978,7 @@
         <v>4.242</v>
       </c>
       <c r="P10" s="11" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="Q10" s="11">
         <v>84464</v>
@@ -2987,7 +2996,7 @@
         <v>4.9</v>
       </c>
       <c r="V10" s="11" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:22" ht="30" customHeight="1">
@@ -3040,7 +3049,7 @@
         <v>7.33</v>
       </c>
       <c r="P11" s="11" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="Q11" s="11">
         <v>21552</v>
@@ -3058,10 +3067,10 @@
         <v>5.7</v>
       </c>
       <c r="V11" s="11" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
-    <row r="12" spans="1:22" ht="30" customHeight="1">
+    <row r="12" spans="1:22" ht="45" customHeight="1">
       <c r="A12" s="11" t="s">
         <v>39</v>
       </c>
@@ -3071,11 +3080,20 @@
       <c r="C12" s="11" t="s">
         <v>41</v>
       </c>
+      <c r="D12" s="11" t="s">
+        <v>42</v>
+      </c>
       <c r="E12" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="H12" s="11">
-        <f>CEILING(BoardQty*2,1)</f>
+        <f>CEILING(BoardQty*2.0,1)</f>
         <v>200</v>
       </c>
       <c r="I12" s="12">
@@ -3089,22 +3107,22 @@
     </row>
     <row r="13" spans="1:22">
       <c r="A13" s="11" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="H13" s="11">
         <f>CEILING(BoardQty*2.0,1)</f>
@@ -3134,7 +3152,7 @@
         <v>3.8</v>
       </c>
       <c r="P13" s="11" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="Q13" s="11">
         <v>28194</v>
@@ -3152,27 +3170,27 @@
         <v>2.8</v>
       </c>
       <c r="V13" s="11" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:22">
       <c r="A14" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="F14" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>47</v>
-      </c>
       <c r="G14" s="11" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H14" s="11">
         <f>CEILING(BoardQty*1.0,1)</f>
@@ -3202,7 +3220,7 @@
         <v>1.25</v>
       </c>
       <c r="P14" s="11" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="Q14" s="11">
         <v>91154</v>
@@ -3220,27 +3238,27 @@
         <v>0.7</v>
       </c>
       <c r="V14" s="11" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:22">
       <c r="A15" s="11" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="H15" s="11">
         <f>CEILING(BoardQty*2.0,1)</f>
@@ -3270,7 +3288,7 @@
         <v>3.8</v>
       </c>
       <c r="P15" s="11" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="Q15" s="11">
         <v>2408384</v>
@@ -3288,27 +3306,27 @@
         <v>2.8</v>
       </c>
       <c r="V15" s="11" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:22">
       <c r="A16" s="11" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="F16" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="G16" s="11" t="s">
         <v>61</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>58</v>
       </c>
       <c r="H16" s="11">
         <f>CEILING(BoardQty*1.0,1)</f>
@@ -3338,7 +3356,7 @@
         <v>14.33</v>
       </c>
       <c r="P16" s="11" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="Q16" s="11">
         <v>11436</v>
@@ -3356,27 +3374,27 @@
         <v>11.8</v>
       </c>
       <c r="V16" s="11" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:22">
       <c r="A17" s="11" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B17" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="F17" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="E17" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>61</v>
-      </c>
       <c r="G17" s="11" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H17" s="11">
         <f>CEILING(BoardQty*1.0,1)</f>
@@ -3406,7 +3424,7 @@
         <v>14.33</v>
       </c>
       <c r="P17" s="11" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="Q17" s="11">
         <v>26927</v>
@@ -3424,30 +3442,30 @@
         <v>12.4</v>
       </c>
       <c r="V17" s="11" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:22" ht="30" customHeight="1">
       <c r="A18" s="11" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E18" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="G18" s="11" t="s">
         <v>69</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>66</v>
       </c>
       <c r="H18" s="11">
         <f>CEILING(BoardQty*2.0,1)</f>
@@ -3477,10 +3495,10 @@
         <v/>
       </c>
       <c r="P18" s="11" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="Q18" s="14" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="R18" s="11"/>
       <c r="S18" s="12">
@@ -3495,30 +3513,30 @@
         <v/>
       </c>
       <c r="V18" s="11" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:22" ht="30" customHeight="1">
       <c r="A19" s="11" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F19" s="11" t="s">
         <v>37</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H19" s="11">
         <f>CEILING(BoardQty*1.0,1)</f>
@@ -3548,7 +3566,7 @@
         <v>12.09</v>
       </c>
       <c r="P19" s="11" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="Q19" s="11">
         <v>149508</v>
@@ -3566,27 +3584,27 @@
         <v>7.0</v>
       </c>
       <c r="V19" s="11" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:22" ht="30" customHeight="1">
       <c r="A20" s="11" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="H20" s="11">
         <f>CEILING(BoardQty*1.0,1)</f>
@@ -3616,7 +3634,7 @@
         <v>422.5</v>
       </c>
       <c r="P20" s="11" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="Q20" s="11">
         <v>4302</v>
@@ -3634,30 +3652,30 @@
         <v>425.0</v>
       </c>
       <c r="V20" s="11" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:22" ht="30" customHeight="1">
       <c r="A21" s="11" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="H21" s="11">
         <f>CEILING(BoardQty*1.0,1)</f>
@@ -3687,7 +3705,7 @@
         <v>22.84</v>
       </c>
       <c r="P21" s="11" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="Q21" s="11">
         <v>3935</v>
@@ -3705,19 +3723,19 @@
         <v>22.5</v>
       </c>
       <c r="V21" s="11" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:22">
       <c r="I23" s="1" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="J23" s="5">
         <f>SUM(O23,U23)</f>
         <v>0</v>
       </c>
       <c r="K23" s="15" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="L23" s="6">
         <f>IFERROR(IF(COUNTIF(L7:L21,"&gt;0")&gt;0,COUNTIF(L7:L21,"&gt;0")&amp;" of "&amp;(ROWS(N7:N21)-COUNTBLANK(N7:N21))&amp;" parts purchased",""),"")</f>
@@ -3728,7 +3746,7 @@
         <v>0</v>
       </c>
       <c r="Q23" s="15" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="R23" s="6">
         <f>IFERROR(IF(COUNTIF(R7:R21,"&gt;0")&gt;0,COUNTIF(R7:R21,"&gt;0")&amp;" of "&amp;(ROWS(T7:T21)-COUNTBLANK(T7:T21))&amp;" parts purchased",""),"")</f>
@@ -3741,10 +3759,10 @@
     </row>
     <row r="24" spans="1:22">
       <c r="A24" s="2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="I24" s="16" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="L24" s="17">
         <f>CONCATENATE(L40,L41,L42,L43,L44,L45,L46,L47,L48,L49,L50,L51,L52,L53,L54)</f>
@@ -4694,37 +4712,38 @@
     <hyperlink ref="G11" r:id="rId12"/>
     <hyperlink ref="P11" r:id="rId13"/>
     <hyperlink ref="V11" r:id="rId14"/>
-    <hyperlink ref="G13" r:id="rId15"/>
-    <hyperlink ref="P13" r:id="rId16"/>
-    <hyperlink ref="V13" r:id="rId17"/>
-    <hyperlink ref="G14" r:id="rId18"/>
-    <hyperlink ref="P14" r:id="rId19"/>
-    <hyperlink ref="V14" r:id="rId20"/>
-    <hyperlink ref="G15" r:id="rId21"/>
-    <hyperlink ref="P15" r:id="rId22"/>
-    <hyperlink ref="V15" r:id="rId23"/>
-    <hyperlink ref="G16" r:id="rId24"/>
-    <hyperlink ref="P16" r:id="rId25"/>
-    <hyperlink ref="V16" r:id="rId26"/>
-    <hyperlink ref="G17" r:id="rId27"/>
-    <hyperlink ref="P17" r:id="rId28"/>
-    <hyperlink ref="V17" r:id="rId29"/>
-    <hyperlink ref="G18" r:id="rId30"/>
-    <hyperlink ref="P18" r:id="rId31"/>
-    <hyperlink ref="V18" r:id="rId32"/>
-    <hyperlink ref="G19" r:id="rId33"/>
-    <hyperlink ref="P19" r:id="rId34"/>
-    <hyperlink ref="V19" r:id="rId35"/>
-    <hyperlink ref="G20" r:id="rId36"/>
-    <hyperlink ref="P20" r:id="rId37"/>
-    <hyperlink ref="V20" r:id="rId38"/>
-    <hyperlink ref="G21" r:id="rId39"/>
-    <hyperlink ref="P21" r:id="rId40"/>
-    <hyperlink ref="V21" r:id="rId41"/>
-    <hyperlink ref="K23" r:id="rId42"/>
-    <hyperlink ref="Q23" r:id="rId43"/>
+    <hyperlink ref="G12" r:id="rId15"/>
+    <hyperlink ref="G13" r:id="rId16"/>
+    <hyperlink ref="P13" r:id="rId17"/>
+    <hyperlink ref="V13" r:id="rId18"/>
+    <hyperlink ref="G14" r:id="rId19"/>
+    <hyperlink ref="P14" r:id="rId20"/>
+    <hyperlink ref="V14" r:id="rId21"/>
+    <hyperlink ref="G15" r:id="rId22"/>
+    <hyperlink ref="P15" r:id="rId23"/>
+    <hyperlink ref="V15" r:id="rId24"/>
+    <hyperlink ref="G16" r:id="rId25"/>
+    <hyperlink ref="P16" r:id="rId26"/>
+    <hyperlink ref="V16" r:id="rId27"/>
+    <hyperlink ref="G17" r:id="rId28"/>
+    <hyperlink ref="P17" r:id="rId29"/>
+    <hyperlink ref="V17" r:id="rId30"/>
+    <hyperlink ref="G18" r:id="rId31"/>
+    <hyperlink ref="P18" r:id="rId32"/>
+    <hyperlink ref="V18" r:id="rId33"/>
+    <hyperlink ref="G19" r:id="rId34"/>
+    <hyperlink ref="P19" r:id="rId35"/>
+    <hyperlink ref="V19" r:id="rId36"/>
+    <hyperlink ref="G20" r:id="rId37"/>
+    <hyperlink ref="P20" r:id="rId38"/>
+    <hyperlink ref="V20" r:id="rId39"/>
+    <hyperlink ref="G21" r:id="rId40"/>
+    <hyperlink ref="P21" r:id="rId41"/>
+    <hyperlink ref="V21" r:id="rId42"/>
+    <hyperlink ref="K23" r:id="rId43"/>
+    <hyperlink ref="Q23" r:id="rId44"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId44"/>
+  <legacyDrawing r:id="rId45"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Use 74AHCT1G14 for better signal level margins
</commit_message>
<xml_diff>
--- a/hardware/documentation/reDIP-RIOT-BOM.xlsx
+++ b/hardware/documentation/reDIP-RIOT-BOM.xlsx
@@ -1287,13 +1287,13 @@
           <t>Qty/Price Breaks (USD):
   Qty  -  Unit$  -  Ext$
 ================
-     1   $0.28      $0.28
-    10   $0.23      $2.28
-    25   $0.19      $4.77
-   100   $0.12     $12.09
-   250   $0.09     $23.33
-   500   $0.08     $39.77
-  1000   $0.05     $54.09</t>
+     1   $0.27      $0.27
+    10   $0.22      $2.23
+    25   $0.19      $4.66
+   100   $0.12     $11.80
+   250   $0.09     $22.78
+   500   $0.08     $38.82
+  1000   $0.05     $52.80</t>
         </r>
       </text>
     </comment>
@@ -1306,7 +1306,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Desc: IC INVERT SCHMITT 1CH 1IN SOT353
+          <t>Desc: IC INVERTER 1CH 1-INP SOT353
 Footprint: 5-TSSOP, SC-70-5, SOT-353</t>
         </r>
       </text>
@@ -1320,7 +1320,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>149508 In Stock</t>
+          <t>1287 In Stock</t>
         </r>
       </text>
     </comment>
@@ -1336,12 +1336,13 @@
           <t>Qty/Price Breaks (USD):
   Qty  -  Unit$  -  Ext$
 ================
-     1   $0.21      $0.21
-    10   $0.14      $1.38
-   100   $0.07      $7.00
-  1000   $0.05     $49.00
-  3000   $0.04    $105.00
-  9000   $0.03    $279.00
+     1   $0.27      $0.27
+    10   $0.18      $1.84
+   100   $0.08      $7.70
+  1000   $0.05     $52.00
+  3000   $0.04    $123.00
+  9000   $0.03    $306.00
+ 24000   $0.03    $768.00
  45000   $0.03  $1,350.00</t>
         </r>
       </text>
@@ -1355,7 +1356,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Desc: Inverters 1-INPUT SCHMITT TR INVERTER 2.0 to 5.5V</t>
+          <t>Desc: Inverters AHC TTL Compatible LOGIC</t>
         </r>
       </text>
     </comment>
@@ -1808,19 +1809,19 @@
     <t>U5</t>
   </si>
   <si>
-    <t>74AHC1G14</t>
+    <t>74AHCT1G14</t>
   </si>
   <si>
     <t>IC SCHMITT-TRIGGER INVERTER</t>
   </si>
   <si>
-    <t>Replacement parts: 74AHC1G14 SOT-353/SC-70-5</t>
+    <t>Replacement parts: 74AHCT1G14 SOT-353/SC-70-5</t>
   </si>
   <si>
     <t>SOT-353_SC-70-5</t>
   </si>
   <si>
-    <t>74AHC1G14SE-7</t>
+    <t>74AHCT1G14SE-7</t>
   </si>
   <si>
     <t>U6</t>
@@ -1907,7 +1908,7 @@
     <t>2156-SN74CBT16210CDGGR-ND</t>
   </si>
   <si>
-    <t>74AHC1G14SE-7DICT-ND</t>
+    <t>74AHCT1G14SE-7DICT-ND</t>
   </si>
   <si>
     <t>220-2155-1-ND</t>
@@ -1958,7 +1959,7 @@
     <t>595-SN74CBT16210CDGG</t>
   </si>
   <si>
-    <t>621-74AHC1G14SE-7</t>
+    <t>621-74AHCT1G14SE-7</t>
   </si>
   <si>
     <t>842-ICE5LP1K-SG48ITR</t>
@@ -1988,7 +1989,7 @@
     <t>Prj date:</t>
   </si>
   <si>
-    <t>on. 04. okt. 2023 kl. 15.15 +0200</t>
+    <t>fr. 06. okt. 2023 kl. 12.39 +0200</t>
   </si>
   <si>
     <t>Board Qty:</t>
@@ -2003,7 +2004,7 @@
     <t>$ date:</t>
   </si>
   <si>
-    <t>2023-10-04 15:15:30</t>
+    <t>2023-10-06 12:40:02</t>
   </si>
   <si>
     <t>KiCost® v1.1.18</t>
@@ -2593,7 +2594,7 @@
       </c>
       <c r="J2" s="4">
         <f>TotalCost/BoardQty</f>
-        <v>5.209</v>
+        <v>5.216</v>
       </c>
     </row>
     <row r="3" spans="1:22">
@@ -2608,11 +2609,11 @@
       </c>
       <c r="J3" s="5">
         <f>SUM(J7:J21)</f>
-        <v>520.902</v>
+        <v>521.602</v>
       </c>
       <c r="O3" s="5">
         <f>SUM(O7:O21)</f>
-        <v>539.732</v>
+        <v>539.442</v>
       </c>
       <c r="P3" s="6" t="str">
         <f>(COUNTA(O7:O21)&amp;" of "&amp;ROWS(O7:O21)&amp;" parts found")</f>
@@ -2620,7 +2621,7 @@
       </c>
       <c r="U3" s="5">
         <f>SUM(U7:U21)</f>
-        <v>524.2</v>
+        <v>524.9</v>
       </c>
       <c r="V3" s="6" t="str">
         <f>(COUNTA(U7:U21)&amp;" of "&amp;ROWS(U7:U21)&amp;" parts found")</f>
@@ -3544,44 +3545,44 @@
       </c>
       <c r="I19" s="12">
         <f>IF(MIN(M19,S19)&lt;&gt;0,MIN(M19,S19),"")</f>
-        <v>0.07</v>
+        <v>0.077</v>
       </c>
       <c r="J19" s="13">
         <f>IF(AND(ISNUMBER(H19),ISNUMBER(I19)),H19*I19,"")</f>
-        <v>7.0</v>
+        <v>7.7</v>
       </c>
       <c r="K19" s="11">
-        <v>315158</v>
+        <v>74194</v>
       </c>
       <c r="L19" s="11"/>
       <c r="M19" s="12">
-        <f>IFERROR(IF(OR(L19&gt;=N19,H19&gt;=N19),LOOKUP(IF(L19="",H19,L19),{0,1,10,25,100,250,500,1000},{0.0,0.28,0.228,0.1908,0.1209,0.09332,0.07954,0.05409}),"MOQ="&amp;N19),"")</f>
-        <v>0.1209</v>
+        <f>IFERROR(IF(OR(L19&gt;=N19,H19&gt;=N19),LOOKUP(IF(L19="",H19,L19),{0,1,10,25,100,250,500,1000},{0.0,0.27,0.223,0.1864,0.118,0.09112,0.07764,0.0528}),"MOQ="&amp;N19),"")</f>
+        <v>0.118</v>
       </c>
       <c r="N19" s="11">
         <v>1</v>
       </c>
       <c r="O19" s="13">
         <f>IFERROR(IF(L19="",H19,L19)*M19,"")</f>
-        <v>12.09</v>
+        <v>11.8</v>
       </c>
       <c r="P19" s="11" t="s">
         <v>108</v>
       </c>
       <c r="Q19" s="11">
-        <v>149508</v>
+        <v>1287</v>
       </c>
       <c r="R19" s="11"/>
       <c r="S19" s="12">
-        <f>IFERROR(IF(OR(R19&gt;=T19,H19&gt;=T19),LOOKUP(IF(R19="",H19,R19),{0,1,10,100,1000,3000,9000,45000},{0.0,0.209,0.138,0.07,0.049,0.035,0.031,0.03}),"MOQ="&amp;T19),"")</f>
-        <v>0.07</v>
+        <f>IFERROR(IF(OR(R19&gt;=T19,H19&gt;=T19),LOOKUP(IF(R19="",H19,R19),{0,1,10,100,1000,3000,9000,24000,45000},{0.0,0.269,0.184,0.077,0.052,0.041,0.034,0.032,0.03}),"MOQ="&amp;T19),"")</f>
+        <v>0.077</v>
       </c>
       <c r="T19" s="11">
         <v>1</v>
       </c>
       <c r="U19" s="13">
         <f>IFERROR(IF(R19="",H19,R19)*S19,"")</f>
-        <v>7.0</v>
+        <v>7.7</v>
       </c>
       <c r="V19" s="11" t="s">
         <v>125</v>

</xml_diff>

<commit_message>
Replaced iCE5LP1K with iCE40UP5K
The MOS 6530 and MOS 6532 have on-chip data port pull-up resistors
in the range of 5k.

While the iCE40UP5K features configurable 3.3k/6.8k/10k/100k pull-up
resistors, the iCE5LP1K only features 100k pull-up resistors.

We make the simple fix of using the more capable (and somewhat more
expensive) pin compatible iCE40UP5K, instead of adding physical
pull-up resistors to separate boards for the MOS 6530 and MOS 6532.
</commit_message>
<xml_diff>
--- a/hardware/documentation/reDIP-RIOT-BOM.xlsx
+++ b/hardware/documentation/reDIP-RIOT-BOM.xlsx
@@ -1360,6 +1360,19 @@
         </r>
       </text>
     </comment>
+    <comment ref="K20" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This part is listed but is not stocked.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="M20" authorId="0">
       <text>
         <r>
@@ -1372,9 +1385,9 @@
           <t>Qty/Price Breaks (USD):
   Qty  -  Unit$  -  Ext$
 ================
-     1   $5.00      $5.00
-    25   $4.35    $108.75
-   100   $4.22    $422.50</t>
+     1  $10.10     $10.10
+    25   $8.80    $220.00
+   100   $8.45    $845.00</t>
         </r>
       </text>
     </comment>
@@ -1401,7 +1414,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>4302 In Stock</t>
+          <t>12647 In Stock</t>
         </r>
       </text>
     </comment>
@@ -1417,10 +1430,10 @@
           <t>Qty/Price Breaks (USD):
   Qty  -  Unit$  -  Ext$
 ================
-     1   $5.03      $5.03
-    25   $4.37    $109.25
-   100   $4.25    $425.00
-  2000   $4.24  $8,480.00</t>
+     1  $10.17     $10.17
+    25   $8.85    $221.25
+   100   $8.50    $850.00
+  2000   $8.50 $17,000.00</t>
         </r>
       </text>
     </comment>
@@ -1433,7 +1446,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Desc: FPGA - Field Programmable Gate Array iCE40 Ultra FPGA 1100 Logic Cells</t>
+          <t>Desc: FPGA - Field Programmable Gate Array iCE40 UltraPlus, 5280 LUTs, 1.2V</t>
         </r>
       </text>
     </comment>
@@ -1581,7 +1594,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="142">
   <si>
     <t>Global Part Info</t>
   </si>
@@ -1827,7 +1840,7 @@
     <t>U6</t>
   </si>
   <si>
-    <t>ICE5LP1K-SG48</t>
+    <t>ICE40UP5K-SG48</t>
   </si>
   <si>
     <t>IC FPGA QFN-48</t>
@@ -1839,7 +1852,7 @@
     <t>Lattice</t>
   </si>
   <si>
-    <t>ICE5LP1K-SG48ITR</t>
+    <t>ICE40UP5K-SG48I</t>
   </si>
   <si>
     <t>U7</t>
@@ -1911,7 +1924,10 @@
     <t>74AHCT1G14SE-7DICT-ND</t>
   </si>
   <si>
-    <t>220-2155-1-ND</t>
+    <t>220-2212-1-ND</t>
+  </si>
+  <si>
+    <t>NonStk</t>
   </si>
   <si>
     <t>1695-AT25EU0011A-SSHN-TCT-ND</t>
@@ -1932,9 +1948,6 @@
     <t>81-GRM035R61A225ME1D</t>
   </si>
   <si>
-    <t>NonStk</t>
-  </si>
-  <si>
     <t>81-GRM033R60J224ME9D</t>
   </si>
   <si>
@@ -1962,7 +1975,7 @@
     <t>621-74AHCT1G14SE-7</t>
   </si>
   <si>
-    <t>842-ICE5LP1K-SG48ITR</t>
+    <t>842-ICE40UP5K-SG48I</t>
   </si>
   <si>
     <t>724-AT25EU0011ASSHNT</t>
@@ -1989,7 +2002,7 @@
     <t>Prj date:</t>
   </si>
   <si>
-    <t>fr. 06. okt. 2023 kl. 12.39 +0200</t>
+    <t>Sat 04 Nov 2023 08:29:48 AM CET</t>
   </si>
   <si>
     <t>Board Qty:</t>
@@ -2004,7 +2017,7 @@
     <t>$ date:</t>
   </si>
   <si>
-    <t>2023-10-06 12:40:02</t>
+    <t>2023-11-04 08:29:49</t>
   </si>
   <si>
     <t>KiCost® v1.1.18</t>
@@ -2594,7 +2607,7 @@
       </c>
       <c r="J2" s="4">
         <f>TotalCost/BoardQty</f>
-        <v>5.216</v>
+        <v>9.441</v>
       </c>
     </row>
     <row r="3" spans="1:22">
@@ -2609,11 +2622,11 @@
       </c>
       <c r="J3" s="5">
         <f>SUM(J7:J21)</f>
-        <v>521.602</v>
+        <v>944.102</v>
       </c>
       <c r="O3" s="5">
         <f>SUM(O7:O21)</f>
-        <v>539.442</v>
+        <v>961.942</v>
       </c>
       <c r="P3" s="6" t="str">
         <f>(COUNTA(O7:O21)&amp;" of "&amp;ROWS(O7:O21)&amp;" parts found")</f>
@@ -2621,7 +2634,7 @@
       </c>
       <c r="U3" s="5">
         <f>SUM(U7:U21)</f>
-        <v>524.9</v>
+        <v>949.9</v>
       </c>
       <c r="V3" s="6" t="str">
         <f>(COUNTA(U7:U21)&amp;" of "&amp;ROWS(U7:U21)&amp;" parts found")</f>
@@ -2658,7 +2671,7 @@
       <c r="O5" s="8"/>
       <c r="P5" s="8"/>
       <c r="Q5" s="9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="R5" s="9"/>
       <c r="S5" s="9"/>
@@ -2802,7 +2815,7 @@
         <v>17.8</v>
       </c>
       <c r="V7" s="11" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:22">
@@ -2873,7 +2886,7 @@
         <v>10.8</v>
       </c>
       <c r="V8" s="11" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:22">
@@ -2911,7 +2924,7 @@
         <v/>
       </c>
       <c r="Q9" s="14" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="R9" s="11"/>
       <c r="S9" s="12">
@@ -2926,7 +2939,7 @@
         <v/>
       </c>
       <c r="V9" s="11" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="45" customHeight="1">
@@ -3499,7 +3512,7 @@
         <v>107</v>
       </c>
       <c r="Q18" s="14" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="R18" s="11"/>
       <c r="S18" s="12">
@@ -3613,44 +3626,44 @@
       </c>
       <c r="I20" s="12">
         <f>IF(MIN(M20,S20)&lt;&gt;0,MIN(M20,S20),"")</f>
-        <v>4.225</v>
+        <v>8.45</v>
       </c>
       <c r="J20" s="13">
         <f>IF(AND(ISNUMBER(H20),ISNUMBER(I20)),H20*I20,"")</f>
-        <v>422.5</v>
-      </c>
-      <c r="K20" s="11">
-        <v>2190</v>
+        <v>845.0</v>
+      </c>
+      <c r="K20" s="14" t="s">
+        <v>110</v>
       </c>
       <c r="L20" s="11"/>
       <c r="M20" s="12">
-        <f>IFERROR(IF(OR(L20&gt;=N20,H20&gt;=N20),LOOKUP(IF(L20="",H20,L20),{0,1,25,100},{0.0,5.0,4.35,4.225}),"MOQ="&amp;N20),"")</f>
-        <v>4.225</v>
+        <f>IFERROR(IF(OR(L20&gt;=N20,H20&gt;=N20),LOOKUP(IF(L20="",H20,L20),{0,1,25,100},{0.0,10.1,8.8,8.45}),"MOQ="&amp;N20),"")</f>
+        <v>8.45</v>
       </c>
       <c r="N20" s="11">
         <v>1</v>
       </c>
       <c r="O20" s="13">
         <f>IFERROR(IF(L20="",H20,L20)*M20,"")</f>
-        <v>422.5</v>
+        <v>845.0</v>
       </c>
       <c r="P20" s="11" t="s">
         <v>109</v>
       </c>
       <c r="Q20" s="11">
-        <v>4302</v>
+        <v>12647</v>
       </c>
       <c r="R20" s="11"/>
       <c r="S20" s="12">
-        <f>IFERROR(IF(OR(R20&gt;=T20,H20&gt;=T20),LOOKUP(IF(R20="",H20,R20),{0,1,25,100,2000},{0.0,5.03,4.37,4.25,4.24}),"MOQ="&amp;T20),"")</f>
-        <v>4.25</v>
+        <f>IFERROR(IF(OR(R20&gt;=T20,H20&gt;=T20),LOOKUP(IF(R20="",H20,R20),{0,1,25,100,2000},{0.0,10.17,8.85,8.5,8.5}),"MOQ="&amp;T20),"")</f>
+        <v>8.5</v>
       </c>
       <c r="T20" s="11">
         <v>1</v>
       </c>
       <c r="U20" s="13">
         <f>IFERROR(IF(R20="",H20,R20)*S20,"")</f>
-        <v>425.0</v>
+        <v>850.0</v>
       </c>
       <c r="V20" s="11" t="s">
         <v>126</v>
@@ -3706,7 +3719,7 @@
         <v>22.84</v>
       </c>
       <c r="P21" s="11" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="Q21" s="11">
         <v>3935</v>
@@ -3736,7 +3749,7 @@
         <v>0</v>
       </c>
       <c r="K23" s="15" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="L23" s="6">
         <f>IFERROR(IF(COUNTIF(L7:L21,"&gt;0")&gt;0,COUNTIF(L7:L21,"&gt;0")&amp;" of "&amp;(ROWS(N7:N21)-COUNTBLANK(N7:N21))&amp;" parts purchased",""),"")</f>
@@ -3747,7 +3760,7 @@
         <v>0</v>
       </c>
       <c r="Q23" s="15" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="R23" s="6">
         <f>IFERROR(IF(COUNTIF(R7:R21,"&gt;0")&gt;0,COUNTIF(R7:R21,"&gt;0")&amp;" of "&amp;(ROWS(T7:T21)-COUNTBLANK(T7:T21))&amp;" parts purchased",""),"")</f>

</xml_diff>